<commit_message>
Directory Changes/ Problems Practice
</commit_message>
<xml_diff>
--- a/Resources/LeetCode/LeetCode Sorted by Score.xlsx
+++ b/Resources/LeetCode/LeetCode Sorted by Score.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kinag\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kinag\Documents\Career\Programming\Resources\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7664C76-F5FF-45DA-92BF-D23F3B3F928C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44954B87-D4FF-45D8-9F79-7B4819DEF016}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4208" uniqueCount="1413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4216" uniqueCount="1413">
   <si>
     <t>#</t>
   </si>
@@ -4700,8 +4700,8 @@
   <dimension ref="A1:R1395"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K1" sqref="K1:K1048576"/>
+      <pane ySplit="2" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L104" sqref="L104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -7282,7 +7282,9 @@
         <v>14</v>
       </c>
       <c r="K55" s="4"/>
-      <c r="L55" s="7"/>
+      <c r="L55" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="M55" s="7"/>
       <c r="N55" s="7"/>
       <c r="O55" s="7"/>
@@ -7327,7 +7329,9 @@
         <v>14</v>
       </c>
       <c r="K56" s="4"/>
-      <c r="L56" s="7"/>
+      <c r="L56" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="M56" s="7"/>
       <c r="N56" s="7"/>
       <c r="O56" s="7"/>
@@ -7372,7 +7376,9 @@
         <v>14</v>
       </c>
       <c r="K57" s="4"/>
-      <c r="L57" s="7"/>
+      <c r="L57" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="M57" s="7"/>
       <c r="N57" s="7"/>
       <c r="O57" s="7"/>
@@ -7419,7 +7425,9 @@
       <c r="K58" s="4">
         <v>1</v>
       </c>
-      <c r="L58" s="7"/>
+      <c r="L58" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="M58" s="7"/>
       <c r="N58" s="7"/>
       <c r="O58" s="7"/>
@@ -7464,7 +7472,9 @@
         <v>14</v>
       </c>
       <c r="K59" s="4"/>
-      <c r="L59" s="7"/>
+      <c r="L59" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="M59" s="7"/>
       <c r="N59" s="7"/>
       <c r="O59" s="7"/>
@@ -7509,7 +7519,9 @@
         <v>14</v>
       </c>
       <c r="K60" s="4"/>
-      <c r="L60" s="7"/>
+      <c r="L60" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="M60" s="7"/>
       <c r="N60" s="7"/>
       <c r="O60" s="7"/>
@@ -7554,7 +7566,9 @@
         <v>14</v>
       </c>
       <c r="K61" s="4"/>
-      <c r="L61" s="7"/>
+      <c r="L61" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="M61" s="7"/>
       <c r="N61" s="7"/>
       <c r="O61" s="7"/>
@@ -7599,7 +7613,9 @@
         <v>14</v>
       </c>
       <c r="K62" s="4"/>
-      <c r="L62" s="7"/>
+      <c r="L62" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="M62" s="7"/>
       <c r="N62" s="7"/>
       <c r="O62" s="7"/>

</xml_diff>

<commit_message>
MAY 16 - LeetCode
</commit_message>
<xml_diff>
--- a/Resources/LeetCode/LeetCode Sorted by Score.xlsx
+++ b/Resources/LeetCode/LeetCode Sorted by Score.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kinag\Documents\Career\Programming\Resources\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44954B87-D4FF-45D8-9F79-7B4819DEF016}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB49C71-BA32-4DF0-8A88-122593457409}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4216" uniqueCount="1413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4221" uniqueCount="1413">
   <si>
     <t>#</t>
   </si>
@@ -4700,8 +4700,8 @@
   <dimension ref="A1:R1395"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L104" sqref="L104"/>
+      <pane ySplit="2" topLeftCell="A224" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L93" sqref="L93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -7662,7 +7662,9 @@
       <c r="K63" s="4">
         <v>1</v>
       </c>
-      <c r="L63" s="7"/>
+      <c r="L63" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="M63" s="7"/>
       <c r="N63" s="7"/>
       <c r="O63" s="7"/>
@@ -7707,7 +7709,9 @@
         <v>14</v>
       </c>
       <c r="K64" s="4"/>
-      <c r="L64" s="7"/>
+      <c r="L64" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="M64" s="7"/>
       <c r="N64" s="7"/>
       <c r="O64" s="7"/>
@@ -7752,7 +7756,9 @@
         <v>14</v>
       </c>
       <c r="K65" s="4"/>
-      <c r="L65" s="7"/>
+      <c r="L65" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="M65" s="7"/>
       <c r="N65" s="7"/>
       <c r="O65" s="7"/>
@@ -7844,7 +7850,9 @@
         <v>14</v>
       </c>
       <c r="K67" s="4"/>
-      <c r="L67" s="7"/>
+      <c r="L67" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="M67" s="7"/>
       <c r="N67" s="7"/>
       <c r="O67" s="7"/>
@@ -8116,7 +8124,9 @@
         <v>14</v>
       </c>
       <c r="K73" s="4"/>
-      <c r="L73" s="7"/>
+      <c r="L73" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="M73" s="7"/>
       <c r="N73" s="7"/>
       <c r="O73" s="7"/>

</xml_diff>